<commit_message>
Created page navigate button
Page navigate button partially works.
</commit_message>
<xml_diff>
--- a/information.xlsx
+++ b/information.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\VidPlayer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{65DB676C-E024-4C45-BE9D-DF2AED95B772}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7CE244A1-9120-4BBD-AC56-3D91F9C68BFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C0F5CFC3-B38F-45A7-BB7D-4F4BEB487E72}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{C0F5CFC3-B38F-45A7-BB7D-4F4BEB487E72}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="index.html" sheetId="7" r:id="rId1"/>
+    <sheet name="episode.html" sheetId="6" r:id="rId2"/>
+    <sheet name="movies.html" sheetId="5" r:id="rId3"/>
+    <sheet name="anime.html" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="113" uniqueCount="77">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="278" uniqueCount="75">
   <si>
     <t>Name</t>
   </si>
@@ -184,12 +187,6 @@
   </si>
   <si>
     <t>Type</t>
-  </si>
-  <si>
-    <t>Anime</t>
-  </si>
-  <si>
-    <t>Movies</t>
   </si>
   <si>
     <t>Flipped</t>
@@ -637,11 +634,88 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{072697F6-9016-45E4-AB98-6151F0DE07D3}">
-  <dimension ref="A1:I14"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B165540B-F686-4A0F-B782-C19B4FB4F401}">
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.54296875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="6.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1796875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="255.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H9" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACFBC2AC-6DFD-4D27-863A-DCF1007294E9}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -688,6 +762,994 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I9" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEE198DA-383E-48B4-B45E-BE1E07F7E58F}">
+  <dimension ref="A1:H34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.54296875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="6.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1796875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="255.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2019</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2012</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2015</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2018</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2019</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2018</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2010</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2018</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2014</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2017</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2019</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3">
+        <v>2019</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2012</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="3">
+        <v>2015</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2018</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2019</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="3">
+        <v>2018</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="3">
+        <v>2010</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2018</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2014</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2017</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="3">
+        <v>2019</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2019</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="3">
+        <v>2012</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2015</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="3">
+        <v>2018</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="3">
+        <v>2019</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="3">
+        <v>2018</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="3">
+        <v>2010</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2018</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="3">
+        <v>2014</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="3">
+        <v>2017</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="3">
+        <v>2019</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{072697F6-9016-45E4-AB98-6151F0DE07D3}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.54296875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="6.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1796875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="255.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -701,22 +1763,19 @@
         <v>46</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -730,339 +1789,35 @@
         <v>46</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3">
-        <v>2019</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="3">
-        <v>2012</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3">
-        <v>2015</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="3">
-        <v>2018</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="3">
-        <v>2019</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="3">
-        <v>2018</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="3">
-        <v>2010</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="3">
-        <v>2018</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="3">
-        <v>2014</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="3">
-        <v>2017</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="3">
-        <v>2019</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>74</v>
-      </c>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Page buttons fully functional
</commit_message>
<xml_diff>
--- a/information.xlsx
+++ b/information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\VidPlayer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7CE244A1-9120-4BBD-AC56-3D91F9C68BFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{93ABC565-8AA8-49C4-8B5D-4A0815117952}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{C0F5CFC3-B38F-45A7-BB7D-4F4BEB487E72}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="278" uniqueCount="75">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="124" uniqueCount="75">
   <si>
     <t>Name</t>
   </si>
@@ -793,10 +793,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEE198DA-383E-48B4-B45E-BE1E07F7E58F}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1125,576 +1125,77 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="3">
-        <v>2019</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="3">
-        <v>2012</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="3">
-        <v>2015</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="3">
-        <v>2018</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="3">
-        <v>2019</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="3">
-        <v>2018</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="3">
-        <v>2010</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="3">
-        <v>2018</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="3">
-        <v>2014</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="3">
-        <v>2017</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" s="3">
-        <v>2019</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="3">
-        <v>2019</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="3">
-        <v>2012</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="3">
-        <v>2015</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="3">
-        <v>2018</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="3">
-        <v>2019</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="3">
-        <v>2018</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C30" s="3">
-        <v>2010</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" s="3">
-        <v>2018</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C32" s="3">
-        <v>2014</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" s="3">
-        <v>2017</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C34" s="3">
-        <v>2019</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>72</v>
-      </c>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H18" s="1"/>
+    </row>
+    <row r="24" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H29" s="1"/>
+    </row>
+    <row r="35" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H40" s="1"/>
+    </row>
+    <row r="45" spans="8:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H46" s="1"/>
+    </row>
+    <row r="47" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H47" s="1"/>
+    </row>
+    <row r="48" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H48" s="1"/>
+    </row>
+    <row r="49" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H49" s="1"/>
+    </row>
+    <row r="50" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H50" s="1"/>
+    </row>
+    <row r="51" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H51" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>